<commit_message>
Planes de prueba, plantilla de tareas de la iteración
</commit_message>
<xml_diff>
--- a/Documentos/Tareas/Iteración_6 Registro.xlsx
+++ b/Documentos/Tareas/Iteración_6 Registro.xlsx
@@ -5,10 +5,10 @@
   <workbookPr autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\T-REX\Desktop\ProyectoDesarrolloSW-EQ1\Documentos\Tareas\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mauri\OneDrive\Documentos\ProyectoDesarrolloSW-EQ1\Documentos\Tareas\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{90FAE5B3-A572-49A5-8E36-CCE49B231DA6}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C73FA17C-79DF-42FD-A991-6AB2E7BF9ADD}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="25605" windowHeight="16065" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="170" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="183" uniqueCount="68">
   <si>
     <t>Columna</t>
   </si>
@@ -233,6 +233,9 @@
   </si>
   <si>
     <t>Hecho</t>
+  </si>
+  <si>
+    <t>Correcciones de interfaz de administrar usuarios</t>
   </si>
 </sst>
 </file>
@@ -516,7 +519,7 @@
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="es-ES"/>
+  <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -696,6 +699,9 @@
                 <c:pt idx="27">
                   <c:v>0</c:v>
                 </c:pt>
+                <c:pt idx="28">
+                  <c:v>0</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -945,6 +951,9 @@
                 <c:pt idx="27">
                   <c:v>0</c:v>
                 </c:pt>
+                <c:pt idx="28">
+                  <c:v>0</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -1039,6 +1048,39 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="17">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="28">
                   <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
@@ -1166,6 +1208,9 @@
                 </c:pt>
                 <c:pt idx="27">
                   <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>6</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1346,7 +1391,7 @@
                   <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>0</c:v>
+                  <c:v>6</c:v>
                 </c:pt>
                 <c:pt idx="29">
                   <c:v>0</c:v>
@@ -2470,13 +2515,13 @@
   <dimension ref="B1:BA54"/>
   <sheetViews>
     <sheetView tabSelected="1" view="pageBreakPreview" zoomScale="69" zoomScaleSheetLayoutView="69" workbookViewId="0">
-      <pane xSplit="6" ySplit="5" topLeftCell="X6" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="6" ySplit="5" topLeftCell="X12" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="G1" sqref="G1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="AU20" sqref="AU20"/>
+      <selection pane="bottomRight" activeCell="AO37" sqref="AO37"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="10.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="1.42578125" style="2" customWidth="1"/>
     <col min="2" max="2" width="16.42578125" style="2" customWidth="1"/>
@@ -4862,7 +4907,9 @@
       <c r="E24" s="20" t="s">
         <v>41</v>
       </c>
-      <c r="F24" s="20"/>
+      <c r="F24" s="20" t="s">
+        <v>66</v>
+      </c>
       <c r="G24" s="21">
         <v>4</v>
       </c>
@@ -4920,48 +4967,50 @@
         <v>4</v>
       </c>
       <c r="AH24" s="22"/>
-      <c r="AI24" s="22"/>
+      <c r="AI24" s="22">
+        <v>6</v>
+      </c>
       <c r="AJ24" s="22">
         <f t="shared" si="8"/>
-        <v>4</v>
+        <v>-2</v>
       </c>
       <c r="AK24" s="22"/>
       <c r="AL24" s="22"/>
       <c r="AM24" s="22">
         <f t="shared" si="9"/>
-        <v>4</v>
+        <v>-2</v>
       </c>
       <c r="AN24" s="22"/>
       <c r="AO24" s="22"/>
       <c r="AP24" s="22">
         <f t="shared" si="10"/>
-        <v>4</v>
+        <v>-2</v>
       </c>
       <c r="AQ24" s="22"/>
       <c r="AR24" s="22"/>
       <c r="AS24" s="22">
         <f t="shared" si="11"/>
-        <v>4</v>
+        <v>-2</v>
       </c>
       <c r="AT24" s="22"/>
       <c r="AU24" s="22"/>
       <c r="AV24" s="22">
         <f t="shared" si="12"/>
-        <v>4</v>
+        <v>-2</v>
       </c>
       <c r="AW24" s="22"/>
       <c r="AX24" s="22"/>
       <c r="AY24" s="22">
         <f t="shared" si="13"/>
-        <v>4</v>
+        <v>-2</v>
       </c>
       <c r="AZ24" s="22">
         <f t="shared" si="14"/>
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="BA24" s="22">
         <f t="shared" si="15"/>
-        <v>4</v>
+        <v>-2</v>
       </c>
     </row>
     <row r="25" spans="2:53" s="23" customFormat="1" x14ac:dyDescent="0.25">
@@ -4973,7 +5022,9 @@
       <c r="E25" s="20" t="s">
         <v>41</v>
       </c>
-      <c r="F25" s="20"/>
+      <c r="F25" s="20" t="s">
+        <v>66</v>
+      </c>
       <c r="G25" s="21">
         <v>1</v>
       </c>
@@ -5061,18 +5112,20 @@
         <v>1</v>
       </c>
       <c r="AW25" s="22"/>
-      <c r="AX25" s="22"/>
+      <c r="AX25" s="22">
+        <v>1</v>
+      </c>
       <c r="AY25" s="22">
         <f t="shared" ref="AY25" si="174">AV25-AX25</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AZ25" s="22">
         <f t="shared" ref="AZ25" si="175">H25+K25+N25+Q25+T25+W25+Z25+AC25+AF25+AI25+AL25+AO25+AR25+AU25+AX25</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BA25" s="22">
         <f t="shared" ref="BA25" si="176">G25-AZ25</f>
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="26" spans="2:53" s="23" customFormat="1" x14ac:dyDescent="0.25">
@@ -5084,7 +5137,9 @@
       <c r="E26" s="20" t="s">
         <v>41</v>
       </c>
-      <c r="F26" s="20"/>
+      <c r="F26" s="20" t="s">
+        <v>65</v>
+      </c>
       <c r="G26" s="21">
         <v>2</v>
       </c>
@@ -5199,7 +5254,9 @@
       <c r="E27" s="20" t="s">
         <v>41</v>
       </c>
-      <c r="F27" s="20"/>
+      <c r="F27" s="20" t="s">
+        <v>66</v>
+      </c>
       <c r="G27" s="21">
         <v>5</v>
       </c>
@@ -5263,42 +5320,48 @@
         <v>5</v>
       </c>
       <c r="AK27" s="22"/>
-      <c r="AL27" s="22"/>
+      <c r="AL27" s="22">
+        <v>3</v>
+      </c>
       <c r="AM27" s="22">
         <f t="shared" ref="AM27:AM29" si="186">AJ27-AL27</f>
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="AN27" s="22"/>
-      <c r="AO27" s="22"/>
+      <c r="AO27" s="22">
+        <v>4</v>
+      </c>
       <c r="AP27" s="22">
         <f t="shared" ref="AP27:AP29" si="187">AM27-AO27</f>
-        <v>5</v>
+        <v>-2</v>
       </c>
       <c r="AQ27" s="22"/>
-      <c r="AR27" s="22"/>
+      <c r="AR27" s="22">
+        <v>2</v>
+      </c>
       <c r="AS27" s="22">
         <f t="shared" ref="AS27:AS29" si="188">AP27-AR27</f>
-        <v>5</v>
+        <v>-4</v>
       </c>
       <c r="AT27" s="22"/>
       <c r="AU27" s="22"/>
       <c r="AV27" s="22">
         <f t="shared" ref="AV27:AV29" si="189">AS27-AU27</f>
-        <v>5</v>
+        <v>-4</v>
       </c>
       <c r="AW27" s="22"/>
       <c r="AX27" s="22"/>
       <c r="AY27" s="22">
         <f t="shared" ref="AY27:AY29" si="190">AV27-AX27</f>
-        <v>5</v>
+        <v>-4</v>
       </c>
       <c r="AZ27" s="22">
         <f t="shared" ref="AZ27:AZ29" si="191">H27+K27+N27+Q27+T27+W27+Z27+AC27+AF27+AI27+AL27+AO27+AR27+AU27+AX27</f>
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="BA27" s="22">
         <f t="shared" ref="BA27:BA29" si="192">G27-AZ27</f>
-        <v>5</v>
+        <v>-4</v>
       </c>
     </row>
     <row r="28" spans="2:53" s="23" customFormat="1" x14ac:dyDescent="0.25">
@@ -5310,7 +5373,9 @@
       <c r="E28" s="20" t="s">
         <v>41</v>
       </c>
-      <c r="F28" s="20"/>
+      <c r="F28" s="20" t="s">
+        <v>66</v>
+      </c>
       <c r="G28" s="21">
         <v>1</v>
       </c>
@@ -5398,18 +5463,20 @@
         <v>1</v>
       </c>
       <c r="AW28" s="22"/>
-      <c r="AX28" s="22"/>
+      <c r="AX28" s="22">
+        <v>1</v>
+      </c>
       <c r="AY28" s="22">
         <f t="shared" si="190"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AZ28" s="22">
         <f t="shared" si="191"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BA28" s="22">
         <f t="shared" si="192"/>
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="29" spans="2:53" s="23" customFormat="1" x14ac:dyDescent="0.25">
@@ -5421,7 +5488,9 @@
       <c r="E29" s="20" t="s">
         <v>41</v>
       </c>
-      <c r="F29" s="20"/>
+      <c r="F29" s="20" t="s">
+        <v>65</v>
+      </c>
       <c r="G29" s="21">
         <v>2</v>
       </c>
@@ -5536,7 +5605,9 @@
       <c r="E30" s="20" t="s">
         <v>41</v>
       </c>
-      <c r="F30" s="20"/>
+      <c r="F30" s="20" t="s">
+        <v>65</v>
+      </c>
       <c r="G30" s="21">
         <v>4</v>
       </c>
@@ -5647,7 +5718,9 @@
       <c r="E31" s="20" t="s">
         <v>41</v>
       </c>
-      <c r="F31" s="20"/>
+      <c r="F31" s="20" t="s">
+        <v>66</v>
+      </c>
       <c r="G31" s="21">
         <v>1</v>
       </c>
@@ -5735,18 +5808,20 @@
         <v>1</v>
       </c>
       <c r="AW31" s="22"/>
-      <c r="AX31" s="22"/>
+      <c r="AX31" s="22">
+        <v>1</v>
+      </c>
       <c r="AY31" s="22">
         <f t="shared" si="206"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AZ31" s="22">
         <f t="shared" si="207"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BA31" s="22">
         <f t="shared" si="208"/>
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="32" spans="2:53" s="23" customFormat="1" x14ac:dyDescent="0.25">
@@ -5758,7 +5833,9 @@
       <c r="E32" s="20" t="s">
         <v>41</v>
       </c>
-      <c r="F32" s="20"/>
+      <c r="F32" s="20" t="s">
+        <v>65</v>
+      </c>
       <c r="G32" s="21">
         <v>2</v>
       </c>
@@ -5869,7 +5946,9 @@
       <c r="E33" s="20" t="s">
         <v>41</v>
       </c>
-      <c r="F33" s="20"/>
+      <c r="F33" s="20" t="s">
+        <v>66</v>
+      </c>
       <c r="G33" s="21">
         <v>5</v>
       </c>
@@ -5909,171 +5988,187 @@
         <v>5</v>
       </c>
       <c r="Y33" s="22"/>
-      <c r="Z33" s="22"/>
+      <c r="Z33" s="22">
+        <v>3</v>
+      </c>
       <c r="AA33" s="22">
         <f t="shared" si="215"/>
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="AB33" s="22"/>
       <c r="AC33" s="22"/>
       <c r="AD33" s="22">
         <f t="shared" si="216"/>
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="AE33" s="22"/>
-      <c r="AF33" s="22"/>
+      <c r="AF33" s="22">
+        <v>2</v>
+      </c>
       <c r="AG33" s="22">
         <f t="shared" si="217"/>
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="AH33" s="22"/>
-      <c r="AI33" s="22"/>
+      <c r="AI33" s="22">
+        <v>1</v>
+      </c>
       <c r="AJ33" s="22">
         <f t="shared" si="218"/>
-        <v>5</v>
+        <v>-1</v>
       </c>
       <c r="AK33" s="22"/>
       <c r="AL33" s="22"/>
       <c r="AM33" s="22">
         <f t="shared" si="219"/>
-        <v>5</v>
+        <v>-1</v>
       </c>
       <c r="AN33" s="22"/>
       <c r="AO33" s="22"/>
       <c r="AP33" s="22">
         <f t="shared" si="220"/>
-        <v>5</v>
+        <v>-1</v>
       </c>
       <c r="AQ33" s="22"/>
       <c r="AR33" s="22"/>
       <c r="AS33" s="22">
         <f t="shared" si="221"/>
-        <v>5</v>
+        <v>-1</v>
       </c>
       <c r="AT33" s="22"/>
       <c r="AU33" s="22"/>
       <c r="AV33" s="22">
         <f t="shared" si="222"/>
-        <v>5</v>
+        <v>-1</v>
       </c>
       <c r="AW33" s="22"/>
       <c r="AX33" s="22"/>
       <c r="AY33" s="22">
         <f t="shared" si="223"/>
-        <v>5</v>
+        <v>-1</v>
       </c>
       <c r="AZ33" s="22">
         <f t="shared" ref="AZ33" si="225">H33+K33+N33+Q33+T33+W33+Z33+AC33+AF33+AI33+AL33+AO33+AR33+AU33+AX33</f>
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="BA33" s="22">
         <f t="shared" si="224"/>
-        <v>5</v>
+        <v>-1</v>
       </c>
     </row>
-    <row r="34" spans="2:53" x14ac:dyDescent="0.25">
+    <row r="34" spans="2:53" ht="30" x14ac:dyDescent="0.25">
       <c r="B34" s="12"/>
-      <c r="C34" s="5"/>
+      <c r="C34" s="5" t="s">
+        <v>67</v>
+      </c>
       <c r="D34" s="5"/>
-      <c r="E34" s="5"/>
-      <c r="F34" s="5"/>
-      <c r="G34" s="13"/>
+      <c r="E34" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="F34" s="5" t="s">
+        <v>66</v>
+      </c>
+      <c r="G34" s="13">
+        <v>6</v>
+      </c>
       <c r="H34" s="8"/>
       <c r="I34" s="8">
         <f t="shared" si="209"/>
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="J34" s="10"/>
       <c r="K34" s="8"/>
       <c r="L34" s="8">
         <f t="shared" si="210"/>
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="M34" s="10"/>
       <c r="N34" s="8"/>
       <c r="O34" s="8">
         <f t="shared" si="211"/>
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="P34" s="10"/>
       <c r="Q34" s="8"/>
       <c r="R34" s="8">
         <f t="shared" si="212"/>
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="S34" s="10"/>
       <c r="T34" s="8"/>
       <c r="U34" s="8">
         <f t="shared" si="213"/>
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="V34" s="10"/>
       <c r="W34" s="8"/>
       <c r="X34" s="8">
         <f t="shared" si="214"/>
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="Y34" s="10"/>
       <c r="Z34" s="8"/>
       <c r="AA34" s="8">
         <f t="shared" si="215"/>
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="AB34" s="10"/>
       <c r="AC34" s="8"/>
       <c r="AD34" s="8">
         <f t="shared" si="216"/>
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="AE34" s="10"/>
-      <c r="AF34" s="8"/>
+      <c r="AF34" s="8">
+        <v>4</v>
+      </c>
       <c r="AG34" s="8">
         <f t="shared" si="217"/>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AH34" s="10"/>
       <c r="AI34" s="8"/>
       <c r="AJ34" s="8">
         <f t="shared" si="218"/>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AK34" s="10"/>
       <c r="AL34" s="8"/>
       <c r="AM34" s="8">
         <f t="shared" si="219"/>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AN34" s="10"/>
       <c r="AO34" s="8"/>
       <c r="AP34" s="8">
         <f t="shared" si="220"/>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AQ34" s="10"/>
       <c r="AR34" s="8"/>
       <c r="AS34" s="8">
         <f t="shared" si="221"/>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AT34" s="10"/>
       <c r="AU34" s="8"/>
       <c r="AV34" s="8">
         <f t="shared" si="222"/>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AW34" s="10"/>
       <c r="AX34" s="8"/>
       <c r="AY34" s="8">
         <f t="shared" si="223"/>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AZ34" s="8">
         <f>H34+K34+N34+Q34+T34+W34+Z34+AC34+AF34+AI34+AL34+AO34+AR34+AU34+AX34</f>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="BA34" s="8">
         <f t="shared" si="224"/>
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="35" spans="2:53" x14ac:dyDescent="0.25">
@@ -8127,6 +8222,11 @@
     </row>
   </sheetData>
   <mergeCells count="16">
+    <mergeCell ref="AZ4:BA4"/>
+    <mergeCell ref="AO4:AP4"/>
+    <mergeCell ref="AR4:AS4"/>
+    <mergeCell ref="AU4:AV4"/>
+    <mergeCell ref="AX4:AY4"/>
     <mergeCell ref="AL4:AM4"/>
     <mergeCell ref="H4:I4"/>
     <mergeCell ref="K4:L4"/>
@@ -8138,11 +8238,6 @@
     <mergeCell ref="AC4:AD4"/>
     <mergeCell ref="AF4:AG4"/>
     <mergeCell ref="AI4:AJ4"/>
-    <mergeCell ref="AZ4:BA4"/>
-    <mergeCell ref="AO4:AP4"/>
-    <mergeCell ref="AR4:AS4"/>
-    <mergeCell ref="AU4:AV4"/>
-    <mergeCell ref="AX4:AY4"/>
   </mergeCells>
   <pageMargins left="0.62992125984251968" right="0.62992125984251968" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup scale="60" orientation="portrait" r:id="rId1"/>
@@ -8167,7 +8262,7 @@
       <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="10.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="1.42578125" style="4" customWidth="1"/>
     <col min="2" max="2" width="27.7109375" style="4" customWidth="1"/>

</xml_diff>